<commit_message>
Adding Assertion for AddNewContactsPage
</commit_message>
<xml_diff>
--- a/CRMWebAppTest/src/main/java/com/crm/qa/testdata/CrmTestData.xlsx
+++ b/CRMWebAppTest/src/main/java/com/crm/qa/testdata/CrmTestData.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheri\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1306F3A-9397-4099-9021-D40FE985949E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B8BC1791-742E-4AE1-9442-F8160AF92DFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A1CF72BA-5D90-4F42-B5B5-02120E47DEB6}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="22725" windowHeight="15225" xr2:uid="{A1CF72BA-5D90-4F42-B5B5-02120E47DEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="deals" sheetId="2" r:id="rId2"/>
     <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -422,7 +418,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>